<commit_message>
improved logic for background processing ,call rescheduling and hangup
</commit_message>
<xml_diff>
--- a/Hospital_Records.xlsx
+++ b/Hospital_Records.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hospital Records" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hospital_Records" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -425,13 +425,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="25" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="23" customWidth="1" min="3" max="3"/>
     <col width="5" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -460,16 +458,6 @@
           <t>Gender</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Appointment Date</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Visit Reason</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -479,7 +467,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+919049865451</t>
+          <t>+917823844614</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -493,156 +481,81 @@
       <c r="E2" t="inlineStr">
         <is>
           <t>Male</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-06-12</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Routine Checkup</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Priya Sharma</t>
+          <t>Vanshika panjwani</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>+9198459130897</t>
+          <t>+917823844614</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>87 Lajpat Nagar, Delhi</t>
+          <t>24 MG Road, Bengaluru</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-06-13</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Migraine</t>
+          <t>Male</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Rohan Verma</t>
+          <t>Vanshika panjwani</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>+919049865451</t>
+          <t>+917823844614</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>12 Park Street, Kolkata</t>
+          <t>24 MG Road, Bengaluru</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>Male</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-06-14</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Diabetes Follow-up</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sneha Iyer</t>
+          <t>Vanshika panjwani</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>+919049865451</t>
+          <t>+918767545559</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>98 Anna Salai, Chennai</t>
+          <t>24 MG Road, Bengaluru</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2025-06-15</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Thyroid Check</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Vikram Patil</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>+919049865451</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>53 JM Road, Pune</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>39</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
           <t>Male</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2025-06-16</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Back Pain</t>
         </is>
       </c>
     </row>

</xml_diff>